<commit_message>
ajustes nas figuras do grupo 2, solicitado pelo professor
</commit_message>
<xml_diff>
--- a/Data/g2.1.xlsx
+++ b/Data/g2.1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,13 +460,13 @@
         <v>2010</v>
       </c>
       <c r="B2" t="n">
-        <v>4965.067039719723</v>
+        <v>5358.10551236704</v>
       </c>
       <c r="C2" t="n">
-        <v>2003.328241231656</v>
+        <v>1884.314774870098</v>
       </c>
       <c r="D2" t="n">
-        <v>2943.378757288975</v>
+        <v>3461.334214751512</v>
       </c>
     </row>
     <row r="3">
@@ -474,13 +474,13 @@
         <v>2011</v>
       </c>
       <c r="B3" t="n">
-        <v>4639.406138981239</v>
+        <v>5006.665047726751</v>
       </c>
       <c r="C3" t="n">
-        <v>1969.67379414374</v>
+        <v>1852.659666844038</v>
       </c>
       <c r="D3" t="n">
-        <v>2697.353686807661</v>
+        <v>3172.015352190998</v>
       </c>
     </row>
     <row r="4">
@@ -488,13 +488,13 @@
         <v>2012</v>
       </c>
       <c r="B4" t="n">
-        <v>4310.173261815577</v>
+        <v>4651.369846296123</v>
       </c>
       <c r="C4" t="n">
-        <v>1877.294668724669</v>
+        <v>1765.768588620275</v>
       </c>
       <c r="D4" t="n">
-        <v>2476.925999238661</v>
+        <v>2912.798323131551</v>
       </c>
     </row>
     <row r="5">
@@ -502,13 +502,13 @@
         <v>2013</v>
       </c>
       <c r="B5" t="n">
-        <v>4934.777112259634</v>
+        <v>5325.417811275645</v>
       </c>
       <c r="C5" t="n">
-        <v>2070.166972014002</v>
+        <v>1947.18275893511</v>
       </c>
       <c r="D5" t="n">
-        <v>2881.161547800089</v>
+        <v>3388.168450604801</v>
       </c>
     </row>
     <row r="6">
@@ -516,13 +516,13 @@
         <v>2014</v>
       </c>
       <c r="B6" t="n">
-        <v>4833.811158023392</v>
+        <v>5216.459315523864</v>
       </c>
       <c r="C6" t="n">
-        <v>2053.728509237899</v>
+        <v>1931.720870240265</v>
       </c>
       <c r="D6" t="n">
-        <v>2807.440306893804</v>
+        <v>3301.474255074935</v>
       </c>
     </row>
     <row r="7">
@@ -530,13 +530,13 @@
         <v>2015</v>
       </c>
       <c r="B7" t="n">
-        <v>4446.400391192377</v>
+        <v>4798.380818556626</v>
       </c>
       <c r="C7" t="n">
-        <v>1956.591716948743</v>
+        <v>1840.354768007607</v>
       </c>
       <c r="D7" t="n">
-        <v>2542.292994357948</v>
+        <v>2989.66815042156</v>
       </c>
     </row>
     <row r="8">
@@ -544,13 +544,13 @@
         <v>2016</v>
       </c>
       <c r="B8" t="n">
-        <v>3666.81538218903</v>
+        <v>3957.083268959925</v>
       </c>
       <c r="C8" t="n">
-        <v>1754.200754229296</v>
+        <v>1649.987421557196</v>
       </c>
       <c r="D8" t="n">
-        <v>2012.203021318029</v>
+        <v>2366.296606397183</v>
       </c>
     </row>
     <row r="9">
@@ -558,13 +558,13 @@
         <v>2017</v>
       </c>
       <c r="B9" t="n">
-        <v>4545.694115544408</v>
+        <v>4905.534709438249</v>
       </c>
       <c r="C9" t="n">
-        <v>1896.530103925846</v>
+        <v>1783.861287562288</v>
       </c>
       <c r="D9" t="n">
-        <v>2641.208631112659</v>
+        <v>3105.990277509399</v>
       </c>
     </row>
     <row r="10">
@@ -572,13 +572,13 @@
         <v>2018</v>
       </c>
       <c r="B10" t="n">
-        <v>3404.58254044627</v>
+        <v>3674.09187657283</v>
       </c>
       <c r="C10" t="n">
-        <v>1516.957231053735</v>
+        <v>1426.83803107733</v>
       </c>
       <c r="D10" t="n">
-        <v>1919.964961750666</v>
+        <v>2257.82713039374</v>
       </c>
     </row>
     <row r="11">
@@ -586,13 +586,13 @@
         <v>2019</v>
       </c>
       <c r="B11" t="n">
-        <v>4334.525449775204</v>
+        <v>4677.649771924687</v>
       </c>
       <c r="C11" t="n">
-        <v>1763.816253874048</v>
+        <v>1659.031684836401</v>
       </c>
       <c r="D11" t="n">
-        <v>2557.183155595085</v>
+        <v>3007.178579354852</v>
       </c>
     </row>
     <row r="12">
@@ -600,13 +600,13 @@
         <v>2020</v>
       </c>
       <c r="B12" t="n">
-        <v>4683.9703812914</v>
+        <v>5054.757029258187</v>
       </c>
       <c r="C12" t="n">
-        <v>1862.312652032621</v>
+        <v>1751.676621647945</v>
       </c>
       <c r="D12" t="n">
-        <v>2792.128388180006</v>
+        <v>3283.467850698226</v>
       </c>
     </row>
     <row r="13">
@@ -614,13 +614,13 @@
         <v>2021</v>
       </c>
       <c r="B13" t="n">
-        <v>4463.233372877607</v>
+        <v>4816.546311839128</v>
       </c>
       <c r="C13" t="n">
-        <v>1877.547348332924</v>
+        <v>1766.00625707088</v>
       </c>
       <c r="D13" t="n">
-        <v>2594.138789470217</v>
+        <v>3050.637410347314</v>
       </c>
     </row>
     <row r="14">
@@ -628,13 +628,27 @@
         <v>2022</v>
       </c>
       <c r="B14" t="n">
-        <v>4709.16937452569</v>
+        <v>5081.950793909221</v>
       </c>
       <c r="C14" t="n">
-        <v>1945.84360289343</v>
+        <v>1830.245176528996</v>
       </c>
       <c r="D14" t="n">
-        <v>2763.325771632261</v>
+        <v>3249.596748692005</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B15" t="n">
+        <v>5453.00133138303</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1954.835190631959</v>
+      </c>
+      <c r="D15" t="n">
+        <v>3498.166140751071</v>
       </c>
     </row>
   </sheetData>

</xml_diff>